<commit_message>
Revised product and sprint backlog
</commit_message>
<xml_diff>
--- a/docs/Agile Artifacts/Sprint Backlog/USFoodRecall_Sprint_Backlog.xlsx
+++ b/docs/Agile Artifacts/Sprint Backlog/USFoodRecall_Sprint_Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balaji.chode.UBTUS\Documents\GSA18FRFQ\docs\Agile Artifacts\Sprint Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balaji.chode.UBTUS\Documents\USFoodRecall\docs\Agile Artifacts\Sprint Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -654,11 +654,12 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E11:E12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="95" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>